<commit_message>
sua lại chụp màn hình
</commit_message>
<xml_diff>
--- a/report_summary.xlsx
+++ b/report_summary.xlsx
@@ -58,7 +58,7 @@
     <t>SITE_OOS</t>
   </si>
   <si>
-    <t>07/05/2025 13:18:36</t>
+    <t>07/05/2025 14:13:49</t>
   </si>
   <si>
     <t>06/05/2025 23:18:18</t>
@@ -512,7 +512,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="2">
-        <v>0.38</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -538,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="2">
-        <v>14.39</v>
+        <v>15.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>